<commit_message>
Fixed a name in whale wave CLR, added new project for bangarang, started that CLR
</commit_message>
<xml_diff>
--- a/whale-wave/CLR/CLR_whale_wave.xlsx
+++ b/whale-wave/CLR/CLR_whale_wave.xlsx
@@ -2095,10 +2095,11 @@
     <t>2016</t>
   </si>
   <si>
-    <t>Using 10 years of whale surveys and a year of oceanographic, ecosystem-level surveying, we investigated the mechanisms behind a curious pattern in humpback whale (Megapter novaeangliae) distribution, in which whales use a British Columbia fjord system in a kind of wave, propagating from offshore to inland channels as summer turned to fall.</t>
-  </si>
-  <si>
-    <t>Keen, Eric M. | Wray, Janie | Meuter, Hermann | Thompson, Kim-Ly | Barlow, Jay P. | Picard, Chris P.</t>
+    <t>Keen, Eric M. | Wray, Janie | Meuter, Hermann | Thompson, Kim-Ly | Barlow, Jay P. | Picard, Chris R.</t>
+  </si>
+  <si>
+    <t>Using 10 years of whale surveys and a year of oceanographic, ecosystem-level surveying, we investigated the mechanisms behind a curious pattern in humpback whale (Megapter novaeangliae) distribution, in which whales use a British Columbia fjord system in a kind of wave, propagating from offshore to inland channels as summer turned to fall.
+Metadata were prepared by Eric Keen, &lt;a href="mailto:ekeen@ucsd.edu"&gt;ekeen@ucsd.edu&lt;/a&gt;.</t>
   </si>
 </sst>
 </file>
@@ -3152,8 +3153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3240,7 +3241,7 @@
         <v>632</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>633</v>
@@ -3258,7 +3259,7 @@
         <v>636</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>637</v>

</xml_diff>

<commit_message>
Edited OLR and CLR in response to pre-ingest QA, reconciled subjects
</commit_message>
<xml_diff>
--- a/whale-wave/CLR/CLR_whale_wave.xlsx
+++ b/whale-wave/CLR/CLR_whale_wave.xlsx
@@ -2074,9 +2074,6 @@
     <t>This collection contains the data, R programming files, and detailed protocols for various aspects of analysis for the publication: Keen et al. 2016. "Whale Wave": shifting strategies structure the complex use of critical fjord habitat by humpbacks.</t>
   </si>
   <si>
-    <t>Humpback whale | Whale wave | Habitat use | Habitat model | Gitga'at First Nation</t>
-  </si>
-  <si>
     <t>Kitimat Fjord System</t>
   </si>
   <si>
@@ -2100,6 +2097,9 @@
   <si>
     <t>Using 10 years of whale surveys and a year of oceanographic, ecosystem-level surveying, we investigated the mechanisms behind a curious pattern in humpback whale (Megapter novaeangliae) distribution, in which whales use a British Columbia fjord system in a kind of wave, propagating from offshore to inland channels as summer turned to fall.
 Metadata were prepared by Eric Keen, &lt;a href="mailto:ekeen@ucsd.edu"&gt;ekeen@ucsd.edu&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Humpback whale | Megaptera novaeangliae | Whale wave | Habitat use | Habitat model | Gitga'at First Nation</t>
   </si>
 </sst>
 </file>
@@ -3153,8 +3153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3229,10 +3229,10 @@
         <v>631</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>641</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>642</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>357</v>
@@ -3241,13 +3241,13 @@
         <v>632</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>633</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>634</v>
@@ -3259,19 +3259,19 @@
         <v>636</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="23" t="s">
+        <v>639</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>638</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>640</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed preferred citation from CLR to OLR
</commit_message>
<xml_diff>
--- a/whale-wave/CLR/CLR_whale_wave.xlsx
+++ b/whale-wave/CLR/CLR_whale_wave.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="646">
   <si>
     <t>text</t>
   </si>
@@ -2100,9 +2100,6 @@
   </si>
   <si>
     <t>Humpback whale | Megaptera novaeangliae | Habitat use | Habitat model | Gitga'at First Nation</t>
-  </si>
-  <si>
-    <t>Keen, Eric M; Wray, Janie; Meuter, Hermann; Thompson, Kim-Ly; Barlow, Jay P; Picard, Chris R (2017): Data from: "Whale Wave": shifting strategies structure the complex use of critical fjord habitats by humpbacks. UC San Diego Library Digital Collections.</t>
   </si>
 </sst>
 </file>
@@ -3154,7 +3151,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
@@ -3172,12 +3169,12 @@
     <col min="9" max="9" width="14.85546875" style="3" customWidth="1"/>
     <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" style="3" customWidth="1"/>
-    <col min="12" max="13" width="39.140625" style="3" customWidth="1"/>
-    <col min="14" max="15" width="42.85546875" style="3" customWidth="1"/>
-    <col min="16" max="17" width="44.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="42.85546875" style="3" customWidth="1"/>
+    <col min="15" max="16" width="44.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3215,22 +3212,19 @@
         <v>3</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>351</v>
+        <v>459</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>454</v>
+        <v>628</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>628</v>
-      </c>
-      <c r="Q1" s="16" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3268,18 +3262,15 @@
         <v>644</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="O2" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="O2" s="23" t="s">
         <v>639</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>638</v>
       </c>
     </row>
@@ -3315,7 +3306,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>N1:O1</xm:sqref>
+          <xm:sqref>M1:N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3327,7 +3318,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>L1:M1 P1:Q1</xm:sqref>
+          <xm:sqref>L1 O1:P1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated CLR and OLR to implement QA changes
</commit_message>
<xml_diff>
--- a/whale-wave/CLR/CLR_whale_wave.xlsx
+++ b/whale-wave/CLR/CLR_whale_wave.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="647">
   <si>
     <t>text</t>
   </si>
@@ -2077,9 +2077,6 @@
     <t>Kitimat Fjord System</t>
   </si>
   <si>
-    <t>Keen, EM, Wray, J, Meuter, H, Thompson, K-L, and Picard, CR. (Accepted 2016) "Whale Wave": Shifting strategies structure complex use of critical fjord habitat by fin whales. Marine Ecology Progress Series.</t>
-  </si>
-  <si>
     <t>2005-2014 fieldwork was funded in part by the Save Ours Seas Foundation and Willow Gove Foundation with special thanks to Andy Wright, the Zumwalt family, Julie Walters and Sam Rose. 2015 fieldwork was funded by the Gitga’at First Nation Guardian Watchmen, Canadian Department of Fisheries and Oceans, NSF Graduate Research Fellowship program (DGE-114086), and private donations from the Watson, Ayres, Cunningham, Barlow and Keen families.</t>
   </si>
   <si>
@@ -2095,11 +2092,17 @@
     <t>Keen, Eric M. | Wray, Janie | Meuter, Hermann | Thompson, Kim-Ly | Barlow, Jay P. | Picard, Chris R.</t>
   </si>
   <si>
-    <t>Using 10 years of whale surveys and a year of oceanographic, ecosystem-level surveying, we investigated the mechanisms behind a curious pattern in humpback whale (Megapter novaeangliae) distribution, in which whales use a British Columbia fjord system in a kind of wave, propagating from offshore to inland channels as summer turned to fall.
+    <t>Humpback whale | Megaptera novaeangliae | Habitat use | Habitat model | Gitga'at First Nation</t>
+  </si>
+  <si>
+    <t>Keen, EM, Wray, J, Meuter, H, Thompson, K-L, Barlow, JP, and Picard, CR. (Accepted 2016) "Whale Wave": Shifting strategies structure complex use of critical fjord habitat by fin whales. Marine Ecology Progress Series.</t>
+  </si>
+  <si>
+    <t>Using 10 years of whale surveys and a year of oceanographic, ecosystem-level surveying, we investigated the mechanisms behind a curious pattern in humpback whale (Megaptera novaeangliae) distribution, in which whales use a British Columbia fjord system in a kind of wave, propagating from offshore to inland channels as summer turned to fall.
 Metadata were prepared by Eric Keen, &lt;a href="mailto:ekeen@ucsd.edu"&gt;ekeen@ucsd.edu&lt;/a&gt;.</t>
   </si>
   <si>
-    <t>Humpback whale | Megaptera novaeangliae | Habitat use | Habitat model | Gitga'at First Nation</t>
+    <t>Keen, Eric M; Wray, Janie; Meuter, Hermann; Thompson, Kim-Ly; Barlow, Jay P; Picard, Chris R (2017): Data from: "Whale Wave": shifting strategies structure the complex use of critical fjord habitats by humpbacks. UC San Diego Library Digital Collections.</t>
   </si>
 </sst>
 </file>
@@ -3151,10 +3154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,12 +3172,12 @@
     <col min="9" max="9" width="14.85546875" style="3" customWidth="1"/>
     <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="39.140625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="42.85546875" style="3" customWidth="1"/>
-    <col min="15" max="16" width="44.5703125" style="3" customWidth="1"/>
+    <col min="12" max="13" width="39.140625" style="3" customWidth="1"/>
+    <col min="14" max="15" width="42.85546875" style="3" customWidth="1"/>
+    <col min="16" max="17" width="44.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3212,27 +3215,30 @@
         <v>3</v>
       </c>
       <c r="M1" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>459</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>640</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>641</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>357</v>
@@ -3241,13 +3247,13 @@
         <v>632</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>633</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>634</v>
@@ -3259,19 +3265,22 @@
         <v>636</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>638</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>644</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>639</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -3306,7 +3315,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:N1</xm:sqref>
+          <xm:sqref>N1:O1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3318,7 +3327,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>L1 O1:P1</xm:sqref>
+          <xm:sqref>L1:M1 P1:Q1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>